<commit_message>
added some test cases and pojo classes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/simple.xlsx
+++ b/src/test/resources/testData/simple.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16824" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22104" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="retriveAllCustomers" sheetId="9" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="37">
   <si>
     <t>endPoint</t>
   </si>
@@ -88,13 +88,52 @@
   </si>
   <si>
     <t>test1@gmail.commmmm</t>
+  </si>
+  <si>
+    <t>validateDeleteCustomerAPIOfValidCustomer</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>cus_D8uIyZJZJ2yjas</t>
+  </si>
+  <si>
+    <t>isValidKeyReq</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>validateRetriveCustomersWithInvalidKey</t>
+  </si>
+  <si>
+    <t>get</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>expectedDataSize</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>cus_D9ihuaPWsiQw3K</t>
+  </si>
+  <si>
+    <t>verifyCustomerUsingPOJO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +154,12 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,13 +183,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -494,10 +540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -506,40 +552,48 @@
     <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -550,7 +604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -561,17 +615,17 @@
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -582,7 +636,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -593,17 +647,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -619,8 +673,11 @@
       <c r="E14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -636,9 +693,144 @@
       <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>